<commit_message>
volume formulas for SCA,Shooting,Passing,Dribbling
</commit_message>
<xml_diff>
--- a/office/ActionBoard.xlsx
+++ b/office/ActionBoard.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\okany\Documents\GitHub\football-simulation-game\office\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B8F7B9-736D-495D-A867-6F3316459081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA303CA-1179-4C77-AA9B-30C392DCB873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="2670" windowWidth="23445" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="2970" windowWidth="23445" windowHeight="12960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Columns" sheetId="1" r:id="rId1"/>
-    <sheet name="Tree" sheetId="2" r:id="rId2"/>
+    <sheet name="VolumeAttributes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Columns!$A$5:$D$5</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="209">
   <si>
     <t>defense</t>
   </si>
@@ -609,21 +609,6 @@
     <t>non-penalty gol beklentisi</t>
   </si>
   <si>
-    <t>pas</t>
-  </si>
-  <si>
-    <t>ATAK</t>
-  </si>
-  <si>
-    <t>kontrol</t>
-  </si>
-  <si>
-    <t>top sürme</t>
-  </si>
-  <si>
-    <t>çalım</t>
-  </si>
-  <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
@@ -631,13 +616,64 @@
   </si>
   <si>
     <t>evet</t>
+  </si>
+  <si>
+    <t>OG</t>
+  </si>
+  <si>
+    <t>Recov</t>
+  </si>
+  <si>
+    <t>kendi kalesine gol</t>
+  </si>
+  <si>
+    <t>sahipsiz top kazanma</t>
+  </si>
+  <si>
+    <t>Total_Defensive_Action</t>
+  </si>
+  <si>
+    <t>toplam defans aksiyonu</t>
+  </si>
+  <si>
+    <t>DEFANS ATAĞIN ZITTIDIR</t>
+  </si>
+  <si>
+    <t>Passing</t>
+  </si>
+  <si>
+    <t>Dribbling</t>
+  </si>
+  <si>
+    <t>Shooting</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>attributes</t>
+  </si>
+  <si>
+    <t>['tpr_x', 'Acceleration_x', 'Technique_x', 'Composure_x', 'Finishing_x', 'Heading_x', 'First Touch_x', 'Agility_x', 'Corners_x', 'Long Shots_x', 'Work Rate_x', 'Off the Ball_x', 'Teamwork_x', 'Crossing_x', 'tpr_y', 'Acceleration_y', 'Work Rate_y', 'Agility_y', 'Technique_y', 'Off the Ball_y', 'Marking_y', 'Crossing_y', 'Long Shots_y', 'Teamwork_y', 'Corners_y', 'Decisions_y', 'Positioning_y', 'Finishing_y', 'Balance_y', 'Composure_y']</t>
+  </si>
+  <si>
+    <t>Hava Topu aksiyonların sonucudur</t>
+  </si>
+  <si>
+    <t>['tpr_x', 'Technique_x', 'Composure_x', 'Acceleration_x', 'Anticipation_x', 'Agility_x', 'Tackling_x', 'Teamwork_x', 'Off the Ball_x', 'Decisions_x', 'Work Rate_x', 'Acceleration_y', 'tpr_y', 'Technique_y', 'Composure_y', 'Crossing_y', 'Work Rate_y', 'Decisions_y', 'Agility_y', 'Off the Ball_y', 'Leadership_y', 'Teamwork_y', 'Anticipation_y', 'Tackling_y']</t>
+  </si>
+  <si>
+    <t>['Dribbling_x', 'Technique_x', 'Composure_x', 'Acceleration_x', 'Anticipation_x', 'Balance_x', 'Vision_y', 'Tackling_y', 'Fitness_y', 'Decisions_y', 'Acceleration_y', 'Marking_y', 'Determination_y', 'Work Rate_y', 'Agility_y', 'Positioning_y', 'Concentration_y']</t>
+  </si>
+  <si>
+    <t>['tpr_x', 'Acceleration_x', 'Technique_x', 'Finishing_x', 'Composure_x', 'Agility_x', 'Long Shots_x', 'Off the Ball_x', 'Teamwork_x', 'Work Rate_x', 'First Touch_x', 'tpr_y', 'Acceleration_y', 'Off the Ball_y', 'Agility_y', 'Work Rate_y', 'Decisions_y', 'Teamwork_y', 'Balance_y', 'Positioning_y', 'Marking_y']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -688,8 +724,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -711,12 +754,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -785,17 +822,17 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1077,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:D105"/>
+  <dimension ref="A3:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,20 +1128,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -1116,134 +1153,134 @@
       <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>195</v>
+      <c r="D5" s="12" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>196</v>
+        <v>87</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>19</v>
+      <c r="C8" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>46</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>39</v>
+      <c r="A9" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>62</v>
+      <c r="A10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>85</v>
+        <v>196</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>90</v>
+      <c r="A12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>196</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>158</v>
+        <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>196</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>182</v>
+      <c r="A14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>196</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1531,10 +1568,10 @@
         <v>47</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>46</v>
@@ -1545,10 +1582,10 @@
         <v>47</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>46</v>
@@ -1559,10 +1596,10 @@
         <v>47</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>46</v>
@@ -1573,10 +1610,10 @@
         <v>47</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>46</v>
@@ -1587,10 +1624,10 @@
         <v>47</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>46</v>
@@ -1601,10 +1638,10 @@
         <v>47</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>46</v>
@@ -1615,10 +1652,10 @@
         <v>47</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>46</v>
@@ -1629,10 +1666,10 @@
         <v>47</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>46</v>
@@ -1643,10 +1680,10 @@
         <v>47</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>46</v>
@@ -1657,24 +1694,24 @@
         <v>47</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>46</v>
@@ -1685,10 +1722,10 @@
         <v>69</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>46</v>
@@ -1699,10 +1736,10 @@
         <v>69</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>46</v>
@@ -1713,10 +1750,10 @@
         <v>69</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>46</v>
@@ -1727,10 +1764,10 @@
         <v>69</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>46</v>
@@ -1741,10 +1778,10 @@
         <v>69</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>46</v>
@@ -1755,10 +1792,10 @@
         <v>69</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>46</v>
@@ -1769,52 +1806,52 @@
         <v>69</v>
       </c>
       <c r="B52" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D52" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="D53" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>94</v>
+      <c r="A54" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>194</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>95</v>
+      <c r="A55" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>195</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>46</v>
@@ -1825,10 +1862,10 @@
         <v>89</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>46</v>
@@ -1839,10 +1876,10 @@
         <v>89</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>46</v>
@@ -1853,10 +1890,10 @@
         <v>89</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>46</v>
@@ -1867,10 +1904,10 @@
         <v>89</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>46</v>
@@ -1881,10 +1918,10 @@
         <v>89</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>46</v>
@@ -1895,10 +1932,10 @@
         <v>89</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>46</v>
@@ -1909,10 +1946,10 @@
         <v>89</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>46</v>
@@ -1923,10 +1960,10 @@
         <v>89</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>46</v>
@@ -1937,10 +1974,10 @@
         <v>89</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>46</v>
@@ -1951,10 +1988,10 @@
         <v>89</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>46</v>
@@ -1964,11 +2001,11 @@
       <c r="A66" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>115</v>
+      <c r="B66" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>46</v>
@@ -1979,10 +2016,10 @@
         <v>89</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>46</v>
@@ -1993,10 +2030,10 @@
         <v>89</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>46</v>
@@ -2006,53 +2043,53 @@
       <c r="A69" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>46</v>
@@ -2063,10 +2100,10 @@
         <v>123</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>46</v>
@@ -2077,10 +2114,10 @@
         <v>123</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>46</v>
@@ -2091,10 +2128,10 @@
         <v>123</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>46</v>
@@ -2105,10 +2142,10 @@
         <v>123</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>46</v>
@@ -2119,10 +2156,10 @@
         <v>123</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>46</v>
@@ -2133,10 +2170,10 @@
         <v>123</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>139</v>
+        <v>74</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>46</v>
@@ -2147,10 +2184,10 @@
         <v>123</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>46</v>
@@ -2161,52 +2198,52 @@
         <v>123</v>
       </c>
       <c r="B80" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C83" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>46</v>
@@ -2217,10 +2254,10 @@
         <v>145</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>46</v>
@@ -2231,10 +2268,10 @@
         <v>145</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>46</v>
@@ -2245,10 +2282,10 @@
         <v>145</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>46</v>
@@ -2259,10 +2296,10 @@
         <v>145</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>46</v>
@@ -2273,10 +2310,10 @@
         <v>145</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>46</v>
@@ -2287,10 +2324,10 @@
         <v>145</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>92</v>
+        <v>152</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>46</v>
@@ -2301,10 +2338,10 @@
         <v>145</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>93</v>
+        <v>160</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>46</v>
@@ -2314,11 +2351,11 @@
       <c r="A91" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B91" s="6" t="s">
-        <v>115</v>
+      <c r="B91" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>46</v>
@@ -2329,10 +2366,10 @@
         <v>145</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>46</v>
@@ -2343,10 +2380,10 @@
         <v>145</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>163</v>
+        <v>93</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>46</v>
@@ -2356,11 +2393,11 @@
       <c r="A94" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B94" s="4" t="s">
-        <v>164</v>
+      <c r="B94" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>46</v>
@@ -2371,52 +2408,52 @@
         <v>145</v>
       </c>
       <c r="B95" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B98" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="C98" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D97" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>46</v>
@@ -2427,10 +2464,10 @@
         <v>88</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>126</v>
+        <v>174</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>46</v>
@@ -2441,10 +2478,10 @@
         <v>88</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>46</v>
@@ -2455,10 +2492,10 @@
         <v>88</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>46</v>
@@ -2469,10 +2506,10 @@
         <v>88</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>179</v>
+        <v>126</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>111</v>
+        <v>185</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>46</v>
@@ -2483,30 +2520,56 @@
         <v>88</v>
       </c>
       <c r="B103" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D104" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C106" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D103" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="10"/>
-      <c r="B104" s="10"/>
-      <c r="C104" s="10"/>
-      <c r="D104" s="10"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="2"/>
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
-      <c r="D105" s="2"/>
+      <c r="D106" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:D5" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:D103">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:D106">
       <sortCondition descending="1" ref="D5"/>
     </sortState>
   </autoFilter>
@@ -2520,64 +2583,68 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A5BAB4-6C7D-4CD0-A70F-E83182D5DBAD}">
-  <dimension ref="B6:K26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="13" width="13.140625" customWidth="1"/>
+    <col min="1" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="13" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" t="s">
-        <v>182</v>
-      </c>
-      <c r="I11" t="s">
-        <v>194</v>
-      </c>
       <c r="J11" t="s">
         <v>46</v>
       </c>
@@ -2585,113 +2652,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
statsbomb Pass Locations heatmap
</commit_message>
<xml_diff>
--- a/office/ActionBoard.xlsx
+++ b/office/ActionBoard.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\okany\Documents\GitHub\football-simulation-game\office\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038C6643-2D5E-483A-B1F2-989FFCFB9C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D52076-13FD-4A7E-BE26-96AA0ACC3634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2175" windowWidth="23445" windowHeight="12960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3525" yWindow="2520" windowWidth="23445" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Columns" sheetId="1" r:id="rId1"/>
     <sheet name="VolumeAttributes" sheetId="2" r:id="rId2"/>
     <sheet name="TodoPlanner" sheetId="3" r:id="rId3"/>
+    <sheet name="Tactics" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Columns!$A$5:$D$5</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="216">
   <si>
     <t>defense</t>
   </si>
@@ -683,6 +684,12 @@
   </si>
   <si>
     <t>Getting Players Data (FM23)</t>
+  </si>
+  <si>
+    <t>Data Preprocessing</t>
+  </si>
+  <si>
+    <t>tpr</t>
   </si>
 </sst>
 </file>
@@ -1150,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:D106"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2620,7 +2627,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2705,8 +2712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84AF4724-A6A6-4989-B8E8-EF45680BE833}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2741,13 +2748,31 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>215</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871406DC-F9B7-4A38-9202-C1EF579761F5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>